<commit_message>
Fix "Indiv" to "Indiv1" to prevent warnings
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Configurations/Scenarios.xlsx
+++ b/inst/extdata/examples/TestProject/Configurations/Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\inst\extdata\examples\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A63FBE1-467D-4232-9F55-ECF0D3C7D94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E33441-313A-4F94-9AAC-F6365EC1F184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t>TestScenario2</t>
-  </si>
-  <si>
-    <t>Indiv</t>
   </si>
   <si>
     <t>SteadyStateTime</t>
@@ -524,27 +521,27 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.15625" customWidth="1"/>
-    <col min="2" max="2" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.83984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.15625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.15625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.15625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -552,10 +549,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -573,19 +570,19 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -599,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -608,12 +605,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -622,7 +619,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -634,24 +631,24 @@
         <v>500</v>
       </c>
       <c r="K3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" t="s">
         <v>13</v>
       </c>
       <c r="M3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -663,7 +660,7 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -675,15 +672,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -695,7 +692,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H5" t="s">
         <v>12</v>
@@ -707,21 +704,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -745,34 +742,34 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.26171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>24</v>
       </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -782,17 +779,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1029,6 +1015,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1039,17 +1036,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB9A7DEF-8D50-4222-A255-A8C989265833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1068,6 +1054,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
- Fixes #883 - Parenthesis in parameter sheet names are ignored
</commit_message>
<xml_diff>
--- a/inst/extdata/examples/TestProject/Configurations/Scenarios.xlsx
+++ b/inst/extdata/examples/TestProject/Configurations/Scenarios.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix\Code\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub repositories\ESQlabs\esqlabsR\inst\extdata\examples\TestProject\Configurations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19E33441-313A-4F94-9AAC-F6365EC1F184}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7624E18E-C347-4779-9780-D1D0F60FD85A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="21840" windowHeight="37920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="8" r:id="rId1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>SimulationTime</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>TestScenario_missingParam</t>
+  </si>
+  <si>
+    <t>"Global", "Aciclovir"</t>
   </si>
 </sst>
 </file>
@@ -521,7 +524,7 @@
   <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +616,7 @@
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -779,6 +782,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="17" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b3e823de345af38b5a0fa8b2c9729ead">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7fae56da9623201e330c5b1623e145d1" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1015,17 +1029,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1036,6 +1039,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB9A7DEF-8D50-4222-A255-A8C989265833}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1054,17 +1068,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2633B21-6509-4402-A676-EEE1878D6EA1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46FCC551-4FF5-46A3-9024-D54BBA18C5A1}">
   <ds:schemaRefs>

</xml_diff>